<commit_message>
New tests and testdata files added. This commit has the fix for the failures due to new buttons added on confidential notice page
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/Check_Delete_Button_Enabled_In_Tabbed_View_GF.xlsx
+++ b/src/main/resources/testdata/Check_Delete_Button_Enabled_In_Tabbed_View_GF.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
   <si>
     <t>Data#</t>
   </si>
@@ -85,9 +85,6 @@
   </si>
   <si>
     <t>Gene</t>
-  </si>
-  <si>
-    <t>Click on delete button in confirm delete message</t>
   </si>
   <si>
     <t>addSequence</t>
@@ -187,6 +184,15 @@
   </si>
   <si>
     <t>SELENIUMAAA</t>
+  </si>
+  <si>
+    <t>Check vertically align magnifying glass on literature evidence tab details and trait components for genetic feature</t>
+  </si>
+  <si>
+    <t>addGFSymbol</t>
+  </si>
+  <si>
+    <t>AAP55168</t>
   </si>
 </sst>
 </file>
@@ -528,10 +534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB2"/>
+  <dimension ref="A1:AC2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D2" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -540,10 +546,14 @@
     <col min="2" max="2" width="86.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.140625" customWidth="1"/>
-    <col min="12" max="12" width="44" customWidth="1"/>
+    <col min="6" max="6" width="19.5703125" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" customWidth="1"/>
+    <col min="10" max="11" width="24.85546875" customWidth="1"/>
+    <col min="12" max="12" width="20.28515625" customWidth="1"/>
+    <col min="13" max="13" width="44" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -575,63 +585,66 @@
         <v>11</v>
       </c>
       <c r="K1" t="s">
+        <v>52</v>
+      </c>
+      <c r="L1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" t="s">
         <v>24</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
         <v>25</v>
       </c>
-      <c r="M1" t="s">
-        <v>13</v>
-      </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" t="s">
         <v>26</v>
       </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>27</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>28</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>29</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>30</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>31</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>32</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>33</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>34</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>35</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>36</v>
       </c>
-      <c r="Z1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:28" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" ht="288" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -658,55 +671,58 @@
         <v>20</v>
       </c>
       <c r="K2" t="s">
+        <v>53</v>
+      </c>
+      <c r="L2" t="s">
         <v>21</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="N2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" t="s">
         <v>38</v>
       </c>
-      <c r="M2" t="s">
-        <v>22</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
         <v>39</v>
       </c>
-      <c r="O2" t="s">
+      <c r="Q2" t="s">
         <v>40</v>
       </c>
-      <c r="P2" t="s">
+      <c r="R2" t="s">
         <v>41</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="S2" t="s">
+        <v>50</v>
+      </c>
+      <c r="T2" t="s">
         <v>42</v>
-      </c>
-      <c r="R2" t="s">
-        <v>51</v>
-      </c>
-      <c r="S2" t="s">
-        <v>43</v>
-      </c>
-      <c r="T2" t="s">
-        <v>44</v>
       </c>
       <c r="U2" t="s">
         <v>43</v>
       </c>
       <c r="V2" t="s">
+        <v>42</v>
+      </c>
+      <c r="W2" t="s">
+        <v>44</v>
+      </c>
+      <c r="X2" t="s">
         <v>45</v>
       </c>
-      <c r="W2" t="s">
+      <c r="Y2" t="s">
         <v>46</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Z2" t="s">
         <v>47</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="AA2" t="s">
         <v>48</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AC2" t="s">
         <v>49</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Checking the changes and new test "Check_ThatUserCanSearchByAnAlreadyExist_GF_Name" added.
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/Check_Delete_Button_Enabled_In_Tabbed_View_GF.xlsx
+++ b/src/main/resources/testdata/Check_Delete_Button_Enabled_In_Tabbed_View_GF.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="8025" yWindow="1665" windowWidth="12285" windowHeight="3990"/>
+    <workbookView xWindow="0" yWindow="1125" windowWidth="12765" windowHeight="6210"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -536,8 +537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>